<commit_message>
enable the cond format import test also for xls and xlsx
Change-Id: I04d743ef9f38f4f65ba912f34ac641ea7031aed2
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/formats.xlsx
+++ b/sc/qa/unit/data/xlsx/formats.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="549" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="257" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>text1</t>
   </si>
@@ -27,6 +28,20 @@
     <t>text11</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">text14</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <sz val="10"/>
+        <u val="single"/>
+      </rPr>
+      <t xml:space="preserve"> space</t>
+    </r>
+  </si>
+  <si>
     <t>text2</t>
   </si>
   <si>
@@ -45,6 +60,15 @@
     <t>text13</t>
   </si>
   <si>
+    <t>short col</t>
+  </si>
+  <si>
+    <t>normal col</t>
+  </si>
+  <si>
+    <t>long col</t>
+  </si>
+  <si>
     <t>text4</t>
   </si>
   <si>
@@ -55,27 +79,37 @@
   </si>
   <si>
     <t>text10</t>
+  </si>
+  <si>
+    <t>Hello,
+Calc!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="16">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0.00" numFmtId="165"/>
-    <numFmt formatCode="#,##0.00" numFmtId="166"/>
-    <numFmt formatCode="0.00%" numFmtId="167"/>
-    <numFmt formatCode="0%" numFmtId="168"/>
-    <numFmt formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00" numFmtId="169"/>
-    <numFmt formatCode="0.00E+000" numFmtId="170"/>
-    <numFmt formatCode="0.00E+00" numFmtId="171"/>
-    <numFmt formatCode="# ??/??" numFmtId="172"/>
+    <numFmt formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0" numFmtId="165"/>
+    <numFmt formatCode="# ?/?" numFmtId="166"/>
+    <numFmt formatCode="0.00E+000" numFmtId="167"/>
+    <numFmt formatCode="#,##0\ ;\(#,##0\)" numFmtId="168"/>
+    <numFmt formatCode="#,##0.00\ [$USD];[RED]\-#,##0.00\ [$USD]" numFmtId="169"/>
+    <numFmt formatCode="0%" numFmtId="170"/>
+    <numFmt formatCode="MM/DD/YY" numFmtId="171"/>
+    <numFmt formatCode="HH:MM" numFmtId="172"/>
+    <numFmt formatCode="0.00" numFmtId="173"/>
+    <numFmt formatCode="#,##0.00" numFmtId="174"/>
+    <numFmt formatCode="0.00%" numFmtId="175"/>
+    <numFmt formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00" numFmtId="176"/>
+    <numFmt formatCode="0.00E+00" numFmtId="177"/>
+    <numFmt formatCode="# ??/??" numFmtId="178"/>
+    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="179"/>
   </numFmts>
-  <fonts count="11">
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
+  <fonts count="12">
+    <font>
+      <name val="Arial"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -95,49 +129,47 @@
       <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
+      <name val="Lucida Sans"/>
+      <family val="2"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
       <family val="2"/>
       <color rgb="00000080"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <sz val="10"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
       <family val="2"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <strike val="true"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <i val="true"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
-      <u val="single"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <i val="true"/>
@@ -167,7 +199,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="29">
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -191,43 +223,76 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="167"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="168"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="169"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="170"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="171"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="172"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="173" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="174" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="175" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="170" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="176" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="168" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="170" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="171" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="177" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="178" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="179" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="15">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
     <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
     <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Style1" xfId="20"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Untitled1" xfId="21"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Untitled2" xfId="22"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Untitled3" xfId="23"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Untitled4" xfId="24"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Untitled5" xfId="25"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Untitled6" xfId="26"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Untitled7" xfId="27"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Untitled8" xfId="28"/>
   </cellStyles>
+  <dxfs count="8">
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+    <dxf/>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -243,10 +308,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5764705882353"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="1">
       <c r="A1" s="1" t="n">
         <v>2</v>
       </c>
@@ -287,12 +353,10 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="b">
-        <f aca="false">FALSE()</f>
+      <c r="A6" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="0" t="b">
-        <f aca="false">TRUE()</f>
+      <c r="B6" s="9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -312,69 +376,187 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.01960784313726"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.5607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5764705882353"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="2">
-      <c r="A2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
-      <c r="A3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
+      <c r="C3" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
-      <c r="A4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
-      <c r="A5" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>12</v>
+      <c r="A4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="5">
+      <c r="A5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="6">
+      <c r="D6" s="21" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5764705882353"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="B1" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>12345</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="22" t="n">
+        <v>0.233</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:D1">
+    <cfRule dxfId="0" operator="lessThan" priority="1" type="cellIs">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule dxfId="1" operator="between" priority="2" type="cellIs">
+      <formula>1</formula>
+      <formula>2</formula>
+    </cfRule>
+    <cfRule dxfId="2" operator="greaterThan" priority="3" type="cellIs">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2">
+    <cfRule dxfId="3" operator="expression" priority="1" type="expression">
+      <formula>SUM(E1:E3)</formula>
+    </cfRule>
+    <cfRule dxfId="4" operator="equal" priority="2" type="cellIs">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule dxfId="5" operator="notBetween" priority="3" type="cellIs">
+      <formula>-2</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule dxfId="6" operator="greaterThanOrEqual" priority="4" type="cellIs">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:D2">
+    <cfRule dxfId="7" operator="expression" priority="1" type="expression">
+      <formula>SUM(E1:E3)</formula>
+    </cfRule>
+    <cfRule dxfId="4" operator="equal" priority="2" type="cellIs">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule dxfId="5" operator="notBetween" priority="3" type="cellIs">
+      <formula>-2</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule dxfId="6" operator="greaterThanOrEqual" priority="4" type="cellIs">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
now we can also activate the cond format import test for xlsx
Change-Id: Idb72bb2616c212439241d93ac28c9649457507a3
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/formats.xlsx
+++ b/sc/qa/unit/data/xlsx/formats.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="257" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="257" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -90,15 +90,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="16">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0" numFmtId="165"/>
-    <numFmt formatCode="# ?/?" numFmtId="166"/>
-    <numFmt formatCode="0.00E+000" numFmtId="167"/>
-    <numFmt formatCode="#,##0\ ;\(#,##0\)" numFmtId="168"/>
-    <numFmt formatCode="#,##0.00\ [$USD];[RED]\-#,##0.00\ [$USD]" numFmtId="169"/>
-    <numFmt formatCode="0%" numFmtId="170"/>
-    <numFmt formatCode="MM/DD/YY" numFmtId="171"/>
-    <numFmt formatCode="HH:MM" numFmtId="172"/>
+    <numFmt formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0" numFmtId="164"/>
+    <numFmt formatCode="# ?/?" numFmtId="165"/>
+    <numFmt formatCode="0.00E+000" numFmtId="166"/>
+    <numFmt formatCode="HH:MM" numFmtId="167"/>
+    <numFmt formatCode="#,##0.00\ [$USD];[RED]\-#,##0.00\ [$USD]" numFmtId="168"/>
+    <numFmt formatCode="0%" numFmtId="169"/>
+    <numFmt formatCode="MM/DD/YY" numFmtId="170"/>
+    <numFmt formatCode="#,##0\ ;\(#,##0\)" numFmtId="171"/>
+    <numFmt formatCode="GENERAL" numFmtId="172"/>
     <numFmt formatCode="0.00" numFmtId="173"/>
     <numFmt formatCode="#,##0.00" numFmtId="174"/>
     <numFmt formatCode="0.00%" numFmtId="175"/>
@@ -200,7 +200,7 @@
     </border>
   </borders>
   <cellStyleXfs count="29">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="172">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -223,48 +223,48 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="167"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="171"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="168"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="169"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="170"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="171"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="172"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="167"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="173" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="174" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="175" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="170" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="176" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="177" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="178" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="179" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="172" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="7" numFmtId="172" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="172" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="9" numFmtId="172" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="0">
       <alignment horizontal="justify" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="172" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="172" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="172" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="172" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -284,14 +284,30 @@
     <cellStyle builtinId="54" customBuiltin="true" name="Untitled8" xfId="28"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
-    <dxf/>
+    <dxf>
+      <numFmt formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0" numFmtId="164"/>
+    </dxf>
+    <dxf>
+      <numFmt formatCode="# ?/?" numFmtId="165"/>
+    </dxf>
+    <dxf>
+      <numFmt formatCode="0.00E+000" numFmtId="166"/>
+    </dxf>
+    <dxf>
+      <numFmt formatCode="HH:MM" numFmtId="167"/>
+    </dxf>
+    <dxf>
+      <numFmt formatCode="#,##0.00\ [$USD];[RED]\-#,##0.00\ [$USD]" numFmtId="168"/>
+    </dxf>
+    <dxf>
+      <numFmt formatCode="0%" numFmtId="169"/>
+    </dxf>
+    <dxf>
+      <numFmt formatCode="MM/DD/YY" numFmtId="170"/>
+    </dxf>
+    <dxf>
+      <numFmt formatCode="#,##0\ ;\(#,##0\)" numFmtId="171"/>
+    </dxf>
   </dxfs>
 </styleSheet>
 </file>
@@ -378,7 +394,7 @@
   </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -474,7 +490,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
unit test for  fdo#55198
Change-Id: I15b745366d1f4c3180f44290e72e245f98bbd755
</commit_message>
<xml_diff>
--- a/sc/qa/unit/data/xlsx/formats.xlsx
+++ b/sc/qa/unit/data/xlsx/formats.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -34,6 +35,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <sz val="10"/>
         <u val="single"/>
@@ -89,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="16">
+  <numFmts count="17">
     <numFmt formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0" numFmtId="164"/>
     <numFmt formatCode="# ?/?" numFmtId="165"/>
     <numFmt formatCode="0.00E+000" numFmtId="166"/>
@@ -99,17 +101,19 @@
     <numFmt formatCode="MM/DD/YY" numFmtId="170"/>
     <numFmt formatCode="#,##0\ ;\(#,##0\)" numFmtId="171"/>
     <numFmt formatCode="GENERAL" numFmtId="172"/>
-    <numFmt formatCode="0.00" numFmtId="173"/>
-    <numFmt formatCode="#,##0.00" numFmtId="174"/>
-    <numFmt formatCode="0.00%" numFmtId="175"/>
-    <numFmt formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00" numFmtId="176"/>
-    <numFmt formatCode="0.00E+00" numFmtId="177"/>
-    <numFmt formatCode="# ??/??" numFmtId="178"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="179"/>
+    <numFmt formatCode="D" numFmtId="173"/>
+    <numFmt formatCode="0.00" numFmtId="174"/>
+    <numFmt formatCode="#,##0.00" numFmtId="175"/>
+    <numFmt formatCode="0.00%" numFmtId="176"/>
+    <numFmt formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00" numFmtId="177"/>
+    <numFmt formatCode="0.00E+00" numFmtId="178"/>
+    <numFmt formatCode="# ??/??" numFmtId="179"/>
+    <numFmt formatCode="GENERAL" numFmtId="180"/>
   </numFmts>
   <fonts count="12">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -129,59 +133,74 @@
       <sz val="10"/>
     </font>
     <font>
-      <name val="Lucida Sans"/>
-      <family val="2"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="00404040"/>
+      <sz val="8"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <color rgb="00000080"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
       <u val="single"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <strike val="true"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <i val="true"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <i val="true"/>
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFCC"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -199,7 +218,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="21">
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="172">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -223,27 +242,22 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="171"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="168"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="169"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="170"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="167"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="2" fontId="4" numFmtId="173">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="173" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="174" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="175" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="176" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="169" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="176" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="177" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="177" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="178" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="179" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="180" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="172" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -260,53 +274,194 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="172" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="172" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="11" numFmtId="172" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="172" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="172" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="172" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="173" xfId="20"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="7">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
     <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
     <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
     <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
     <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
     <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Style1" xfId="20"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Untitled1" xfId="21"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Untitled2" xfId="22"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Untitled3" xfId="23"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Untitled4" xfId="24"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Untitled5" xfId="25"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Untitled6" xfId="26"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Untitled7" xfId="27"/>
-    <cellStyle builtinId="54" customBuiltin="true" name="Untitled8" xfId="28"/>
+    <cellStyle builtinId="54" customBuiltin="true" name="Date" xfId="20"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00404040"/>
+    </indexedColors>
+  </colors>
   <dxfs count="8">
     <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </font>
       <numFmt formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0" numFmtId="164"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </font>
       <numFmt formatCode="# ?/?" numFmtId="165"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </font>
       <numFmt formatCode="0.00E+000" numFmtId="166"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </font>
       <numFmt formatCode="HH:MM" numFmtId="167"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </font>
       <numFmt formatCode="#,##0.00\ [$USD];[RED]\-#,##0.00\ [$USD]" numFmtId="168"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </font>
       <numFmt formatCode="0%" numFmtId="169"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </font>
       <numFmt formatCode="MM/DD/YY" numFmtId="170"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </font>
       <numFmt formatCode="#,##0\ ;\(#,##0\)" numFmtId="171"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
 </styleSheet>
@@ -320,15 +475,15 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B5" activeCellId="0" pane="topLeft" sqref="B5"/>
+      <selection activeCell="A5" activeCellId="0" pane="topLeft" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.9" outlineLevel="0" r="1">
       <c r="A1" s="1" t="n">
         <v>2</v>
       </c>
@@ -336,7 +491,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="3" t="n">
         <v>0.401</v>
       </c>
@@ -344,7 +499,7 @@
         <v>-0.2222</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="5" t="n">
         <v>12345</v>
       </c>
@@ -352,7 +507,7 @@
         <v>-1234</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="6" t="n">
         <v>258963</v>
       </c>
@@ -360,7 +515,7 @@
         <v>-2354</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="8" t="n">
         <v>25.378</v>
       </c>
@@ -368,11 +523,13 @@
         <v>0.389</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="A6" s="9" t="b">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="B6" s="9" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -395,18 +552,18 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
+      <selection activeCell="D6" activeCellId="0" pane="topLeft" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.01960784313726"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.5607843137255"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.04705882352941"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.7529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -420,7 +577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.2" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.2" outlineLevel="0" r="2">
       <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
@@ -431,7 +588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
@@ -451,7 +608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="4">
       <c r="A4" s="17" t="s">
         <v>13</v>
       </c>
@@ -459,7 +616,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.9" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.9" outlineLevel="0" r="5">
       <c r="A5" s="19" t="s">
         <v>15</v>
       </c>
@@ -467,7 +624,7 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.85" outlineLevel="0" r="6">
       <c r="D6" s="21" t="s">
         <v>17</v>
       </c>
@@ -475,7 +632,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -495,11 +652,11 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="0" t="n">
         <v>-2</v>
       </c>
@@ -513,7 +670,7 @@
         <v>12345</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="22" t="n">
         <v>0.233</v>
       </c>
@@ -572,10 +729,41 @@
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5764705882353"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
+      <c r="B2" s="23" t="n">
+        <v>24470</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>